<commit_message>
Chỉnh sửa [mô tả phần chỉnh sửa]
</commit_message>
<xml_diff>
--- a/sims.xlsx
+++ b/sims.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="22">
   <si>
     <t>so</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>Lộc phát</t>
+  </si>
+  <si>
+    <t>Vina</t>
+  </si>
+  <si>
+    <t>Tứ quý</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>git commit -m "Chỉnh sửa [mô tả phần chỉnh sửa]"</t>
+  </si>
+  <si>
+    <t>git push origin main</t>
   </si>
 </sst>
 </file>
@@ -417,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +652,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>987585575</v>
+        <v>987580501</v>
       </c>
       <c r="B13">
         <v>1200000</v>
@@ -654,7 +669,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>987585576</v>
+        <v>987580502</v>
       </c>
       <c r="B14">
         <v>1200000</v>
@@ -671,7 +686,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>987585577</v>
+        <v>987580503</v>
       </c>
       <c r="B15">
         <v>1200000</v>
@@ -688,7 +703,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>987585578</v>
+        <v>987580504</v>
       </c>
       <c r="B16">
         <v>1200000</v>
@@ -705,7 +720,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>987585579</v>
+        <v>987580505</v>
       </c>
       <c r="B17">
         <v>1200000</v>
@@ -722,7 +737,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>987585580</v>
+        <v>987580506</v>
       </c>
       <c r="B18">
         <v>1200000</v>
@@ -739,7 +754,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>987585581</v>
+        <v>987580507</v>
       </c>
       <c r="B19">
         <v>1200000</v>
@@ -756,7 +771,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>987585582</v>
+        <v>987580508</v>
       </c>
       <c r="B20">
         <v>1200000</v>
@@ -773,7 +788,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>987585583</v>
+        <v>987580509</v>
       </c>
       <c r="B21">
         <v>1200000</v>
@@ -790,7 +805,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>987585584</v>
+        <v>987580510</v>
       </c>
       <c r="B22">
         <v>1200000</v>
@@ -807,7 +822,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>987585585</v>
+        <v>987580511</v>
       </c>
       <c r="B23">
         <v>1200000</v>
@@ -824,7 +839,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>987585586</v>
+        <v>987580512</v>
       </c>
       <c r="B24">
         <v>1200000</v>
@@ -955,6 +970,312 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>987585574</v>
+      </c>
+      <c r="B32">
+        <v>1200000</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>987585575</v>
+      </c>
+      <c r="B33">
+        <v>1200000</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>987585576</v>
+      </c>
+      <c r="B34">
+        <v>1200000</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>987585577</v>
+      </c>
+      <c r="B35">
+        <v>1200000</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>987585578</v>
+      </c>
+      <c r="B36">
+        <v>1200000</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>987585579</v>
+      </c>
+      <c r="B37">
+        <v>1200000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>987585580</v>
+      </c>
+      <c r="B38">
+        <v>1200000</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>987585581</v>
+      </c>
+      <c r="B39">
+        <v>1200000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>987585582</v>
+      </c>
+      <c r="B40">
+        <v>1200000</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>987585583</v>
+      </c>
+      <c r="B41">
+        <v>1200000</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>987585584</v>
+      </c>
+      <c r="B42">
+        <v>1200000</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>987585585</v>
+      </c>
+      <c r="B43">
+        <v>1200000</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>987585586</v>
+      </c>
+      <c r="B44">
+        <v>1200000</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>987585587</v>
+      </c>
+      <c r="B45">
+        <v>1200000</v>
+      </c>
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>987585588</v>
+      </c>
+      <c r="B46">
+        <v>1200000</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>987585589</v>
+      </c>
+      <c r="B47">
+        <v>1200000</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>987585590</v>
+      </c>
+      <c r="B48">
+        <v>1200000</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>987585591</v>
+      </c>
+      <c r="B49">
+        <v>1200000</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
         <v>10</v>
       </c>
     </row>
@@ -965,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -981,6 +1302,21 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>